<commit_message>
Update the benchmarking sheet
</commit_message>
<xml_diff>
--- a/benchmarking/benchmarks.xlsx
+++ b/benchmarking/benchmarks.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Iteration</t>
   </si>
@@ -39,6 +39,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -48,6 +49,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -57,6 +59,60 @@
   </si>
   <si>
     <t xml:space="preserve">Modified samtools directory for my system</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added subprocesses instead of OS in SamtoText</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added CPU pooling to MakeFullDictionary</t>
   </si>
 </sst>
 </file>
@@ -72,6 +128,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -93,12 +150,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -161,24 +220,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,96 +333,112 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>